<commit_message>
edited typo in flasher_v1_0
</commit_message>
<xml_diff>
--- a/Benchmark Managment/Config.xlsx
+++ b/Benchmark Managment/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyril\Documents\GitHub\P6_Software\Benchmark Managment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\GitHub\P6_Software\Benchmark Managment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C64BDE1-513A-472E-9C46-85EAA7C3B036}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8A4911-EC9C-4CF5-A620-2F44C0A11A75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
   <si>
     <t>Number</t>
   </si>
@@ -211,6 +211,15 @@
   </si>
   <si>
     <t>A2068169</t>
+  </si>
+  <si>
+    <t>master_dfu_package.zip</t>
+  </si>
+  <si>
+    <t>client_dfu_package.zip</t>
+  </si>
+  <si>
+    <t>server_dfu_package.zip</t>
   </si>
 </sst>
 </file>
@@ -282,8 +291,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:D4" totalsRowShown="0">
-  <autoFilter ref="A1:D4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:D6" totalsRowShown="0">
+  <autoFilter ref="A1:D6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Number"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Firmware"/>
@@ -297,8 +306,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabelle2" displayName="Tabelle2" ref="A1:A5" totalsRowShown="0">
-  <autoFilter ref="A1:A5" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabelle2" displayName="Tabelle2" ref="A1:A8" totalsRowShown="0">
+  <autoFilter ref="A1:A8" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Firmware Selection"/>
   </tableColumns>
@@ -590,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -620,47 +629,62 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C2" t="str">
         <f>VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE)</f>
-        <v>A4F21E13</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
+        <v>16D87965</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C3" t="str">
         <f>VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE)</f>
-        <v>E1A6E5BF</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
+        <v>8E323CE7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C4" t="str">
         <f>VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE)</f>
-        <v>A0469D49</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
+        <v>B6D10C96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" t="str">
+        <f>VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE)</f>
+        <v>52993E8A</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" t="str">
+        <f>VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE)</f>
+        <v>6776E907</v>
       </c>
     </row>
   </sheetData>
@@ -673,9 +697,9 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2A9CFBD8-98C6-47B7-83CE-7D8A4658D465}">
           <x14:formula1>
-            <xm:f>Constants!$A$2:$A$5</xm:f>
+            <xm:f>Constants!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B4</xm:sqref>
+          <xm:sqref>B2:B6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -687,13 +711,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -768,6 +792,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
       <c r="C6" s="1">
         <v>5</v>
       </c>
@@ -779,6 +806,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
       <c r="C7" s="1">
         <v>6</v>
       </c>
@@ -790,6 +820,9 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
       <c r="C8" s="1">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Fixed bug in ot_benchmark.py
</commit_message>
<xml_diff>
--- a/Benchmark Managment/Config.xlsx
+++ b/Benchmark Managment/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Raffael\GitHub\P6_Software\Benchmark Managment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\GitHub\P6_Software\Benchmark Managment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B78AD0B-4454-4992-B9FE-CB997D15601A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19733C3-CDD2-415F-8AA4-4A118BFD1901}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2760" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="64">
   <si>
     <t>Number</t>
   </si>
@@ -276,13 +276,13 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="bottom"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -298,8 +298,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:E6" totalsRowShown="0">
-  <autoFilter ref="A1:E6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:E7" totalsRowShown="0">
+  <autoFilter ref="A1:E7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Number"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Firmware"/>
@@ -307,7 +307,7 @@
       <calculatedColumnFormula>VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Group ID"/>
-    <tableColumn id="5" xr3:uid="{BF33E156-0868-4FE7-AEB6-BAA4A1A6CAB8}" name="Node Id" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{BF33E156-0868-4FE7-AEB6-BAA4A1A6CAB8}" name="Node Id" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -327,8 +327,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabelle3" displayName="Tabelle3" ref="C1:D52" totalsRowShown="0">
   <autoFilter ref="C1:D52" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Number" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Device ID" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Number" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Device ID" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -607,22 +607,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -639,95 +639,79 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C2" t="str">
         <f>VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE)</f>
-        <v>7928FDBD</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>E5B83E8E</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C3" t="str">
         <f>VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE)</f>
-        <v>70AAAF03</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>52993E8A</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C4" t="str">
         <f>VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE)</f>
-        <v>5BEB2713</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>228D1458</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5" t="str">
         <f>VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE)</f>
-        <v>EA97A00B</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>B6D10C96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C6" t="str">
         <f>VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE)</f>
-        <v>E22399C0</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0</v>
-      </c>
+        <v>8E323CE7</v>
+      </c>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" t="str">
+        <f>VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE)</f>
+        <v>6776E907</v>
+      </c>
+      <c r="E7" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -741,19 +725,19 @@
           <x14:formula1>
             <xm:f>Constants!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B6</xm:sqref>
+          <xm:sqref>B2:B7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F71A059C-8F2C-4129-B91B-F5697AA9FF5A}">
           <x14:formula1>
             <xm:f>Constants!$C$2:$C$52</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A6</xm:sqref>
+          <xm:sqref>A2:A7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BED282B8-5A63-432E-8F33-CB3377B63A1C}">
           <x14:formula1>
             <xm:f>Constants!$F$2:$F$27</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:E6</xm:sqref>
+          <xm:sqref>D2:E7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -769,13 +753,13 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -789,7 +773,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -803,7 +787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -817,7 +801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -831,7 +815,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -845,7 +829,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -859,7 +843,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -873,7 +857,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -887,7 +871,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C9" s="1">
         <v>8</v>
       </c>
@@ -898,7 +882,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C10" s="1">
         <v>9</v>
       </c>
@@ -909,7 +893,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C11" s="1">
         <v>10</v>
       </c>
@@ -920,7 +904,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C12" s="1">
         <v>11</v>
       </c>
@@ -931,7 +915,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C13" s="1">
         <v>12</v>
       </c>
@@ -942,7 +926,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C14" s="1">
         <v>13</v>
       </c>
@@ -953,7 +937,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C15" s="1">
         <v>14</v>
       </c>
@@ -964,7 +948,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C16" s="1">
         <v>15</v>
       </c>
@@ -975,7 +959,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C17" s="1">
         <v>16</v>
       </c>
@@ -986,7 +970,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C18" s="1">
         <v>17</v>
       </c>
@@ -997,7 +981,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C19" s="1">
         <v>18</v>
       </c>
@@ -1008,7 +992,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C20" s="1">
         <v>19</v>
       </c>
@@ -1019,7 +1003,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C21" s="1">
         <v>20</v>
       </c>
@@ -1030,7 +1014,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C22" s="1">
         <v>21</v>
       </c>
@@ -1041,7 +1025,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C23" s="1">
         <v>22</v>
       </c>
@@ -1052,7 +1036,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C24" s="1">
         <v>23</v>
       </c>
@@ -1063,7 +1047,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C25" s="1">
         <v>24</v>
       </c>
@@ -1074,7 +1058,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C26" s="1">
         <v>25</v>
       </c>
@@ -1085,7 +1069,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C27" s="1">
         <v>26</v>
       </c>
@@ -1096,7 +1080,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C28" s="1">
         <v>27</v>
       </c>
@@ -1104,7 +1088,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C29" s="1">
         <v>28</v>
       </c>
@@ -1112,7 +1096,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C30" s="1">
         <v>29</v>
       </c>
@@ -1120,7 +1104,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C31" s="1">
         <v>30</v>
       </c>
@@ -1128,7 +1112,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C32" s="1">
         <v>31</v>
       </c>
@@ -1136,7 +1120,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C33" s="1">
         <v>32</v>
       </c>
@@ -1144,7 +1128,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C34" s="1">
         <v>33</v>
       </c>
@@ -1152,7 +1136,7 @@
         <v>62688236</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C35" s="1">
         <v>34</v>
       </c>
@@ -1160,7 +1144,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C36" s="1">
         <v>35</v>
       </c>
@@ -1168,7 +1152,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C37" s="1">
         <v>36</v>
       </c>
@@ -1176,7 +1160,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C38" s="1">
         <v>37</v>
       </c>
@@ -1184,7 +1168,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C39" s="1">
         <v>38</v>
       </c>
@@ -1192,7 +1176,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C40" s="1">
         <v>39</v>
       </c>
@@ -1200,7 +1184,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C41" s="1">
         <v>40</v>
       </c>
@@ -1208,7 +1192,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C42" s="1">
         <v>41</v>
       </c>
@@ -1216,7 +1200,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C43" s="1">
         <v>42</v>
       </c>
@@ -1224,7 +1208,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C44" s="1">
         <v>43</v>
       </c>
@@ -1232,7 +1216,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C45" s="1">
         <v>44</v>
       </c>
@@ -1240,7 +1224,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C46" s="1">
         <v>45</v>
       </c>
@@ -1248,7 +1232,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C47" s="1">
         <v>46</v>
       </c>
@@ -1256,7 +1240,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C48" s="1">
         <v>47</v>
       </c>
@@ -1264,7 +1248,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C49" s="1">
         <v>48</v>
       </c>
@@ -1272,7 +1256,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C50" s="1">
         <v>49</v>
       </c>
@@ -1280,7 +1264,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C51" s="1">
         <v>50</v>
       </c>
@@ -1288,7 +1272,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C52" s="1">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
changed zip files for flashing the device
</commit_message>
<xml_diff>
--- a/Benchmark Managment/Config.xlsx
+++ b/Benchmark Managment/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\GitHub\P6_Software\Benchmark Managment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19733C3-CDD2-415F-8AA4-4A118BFD1901}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628B66D5-786C-4F78-94B6-800495E4B67E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-132" yWindow="-132" windowWidth="23304" windowHeight="14664" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
   <si>
     <t>Number</t>
   </si>
@@ -298,8 +298,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:E7" totalsRowShown="0">
-  <autoFilter ref="A1:E7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:E4" totalsRowShown="0">
+  <autoFilter ref="A1:E4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Number"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Firmware"/>
@@ -610,7 +610,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -641,76 +641,44 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" t="str">
         <f>VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE)</f>
-        <v>E5B83E8E</v>
+        <v>8E323CE7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" t="str">
         <f>VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE)</f>
-        <v>52993E8A</v>
+        <v>228D1458</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C4" t="str">
         <f>VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE)</f>
-        <v>228D1458</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" t="str">
-        <f>VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE)</f>
         <v>B6D10C96</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" t="str">
-        <f>VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE)</f>
-        <v>8E323CE7</v>
-      </c>
       <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" t="str">
-        <f>VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE)</f>
-        <v>6776E907</v>
-      </c>
       <c r="E7" s="4"/>
     </row>
   </sheetData>
@@ -725,19 +693,19 @@
           <x14:formula1>
             <xm:f>Constants!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B7</xm:sqref>
+          <xm:sqref>B2:B4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F71A059C-8F2C-4129-B91B-F5697AA9FF5A}">
           <x14:formula1>
             <xm:f>Constants!$C$2:$C$52</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A7</xm:sqref>
+          <xm:sqref>A2:A4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BED282B8-5A63-432E-8F33-CB3377B63A1C}">
           <x14:formula1>
             <xm:f>Constants!$F$2:$F$27</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:E7</xm:sqref>
+          <xm:sqref>D2:E4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>